<commit_message>
make csv from current values
</commit_message>
<xml_diff>
--- a/stroommetingen.xlsx
+++ b/stroommetingen.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\meesj\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\meesj\Documents\GitHub\NSP2_Experiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EEA06F5F-278C-49B5-8A2F-CE563ACDCDDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BBC8F57-C848-416C-9A90-F517CD619576}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{BE825C23-FB4F-400A-91D2-EE38B7C67088}"/>
   </bookViews>
@@ -34,27 +34,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>stroom</t>
-  </si>
-  <si>
-    <t>fout op stroom</t>
-  </si>
-  <si>
-    <t>10 +- 0.03 Hz</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>meting</t>
   </si>
   <si>
-    <t>5, 6</t>
+    <t>current</t>
   </si>
   <si>
-    <t>9, 10</t>
-  </si>
-  <si>
-    <t>fout op functiegenerator freq</t>
+    <t>current_err</t>
   </si>
 </sst>
 </file>
@@ -406,32 +394,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D675C343-52E9-4C53-9B94-8073BDA2E042}">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>4.9000000000000002E-2</v>
       </c>
@@ -443,19 +425,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>0.1</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B17" si="0">IF(A3&lt;0.4, A3 * 0.016 + 4 * 0.00001, A3 * 0.02 + 10 * 0.001)</f>
+        <f t="shared" ref="B3:B16" si="0">IF(A3&lt;0.4, A3 * 0.016 + 4 * 0.00001, A3 * 0.02 + 10 * 0.001)</f>
         <v>1.6400000000000002E-3</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>0.15</v>
       </c>
@@ -467,7 +449,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>0.19900000000000001</v>
       </c>
@@ -479,7 +461,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>0.249</v>
       </c>
@@ -487,127 +469,151 @@
         <f t="shared" si="0"/>
         <v>4.0239999999999998E-3</v>
       </c>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>0.30099999999999999</v>
+        <v>0.249</v>
       </c>
       <c r="B7">
         <f t="shared" si="0"/>
+        <v>4.0239999999999998E-3</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>0.30099999999999999</v>
+      </c>
+      <c r="B8">
+        <f>IF(A8&lt;0.4, A8 * 0.016 + 4 * 0.00001, A8 * 0.02 + 10 * 0.001)</f>
         <v>4.8560000000000001E-3</v>
       </c>
-      <c r="C7">
+      <c r="C8">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9">
         <v>0.35099999999999998</v>
       </c>
-      <c r="B8">
-        <f t="shared" si="0"/>
+      <c r="B9">
+        <f>IF(A9&lt;0.4, A9 * 0.016 + 4 * 0.00001, A9 * 0.02 + 10 * 0.001)</f>
         <v>5.6559999999999996E-3</v>
       </c>
-      <c r="C8">
+      <c r="C9">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10">
         <v>0.40100000000000002</v>
       </c>
-      <c r="B9">
-        <f t="shared" si="0"/>
+      <c r="B10">
+        <f>IF(A10&lt;0.4, A10 * 0.016 + 4 * 0.00001, A10 * 0.02 + 10 * 0.001)</f>
         <v>1.8020000000000001E-2</v>
       </c>
-      <c r="C9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10">
+      <c r="C10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>0.40100000000000002</v>
+      </c>
+      <c r="B11">
+        <f>IF(A11&lt;0.4, A11 * 0.016 + 4 * 0.00001, A11 * 0.02 + 10 * 0.001)</f>
+        <v>1.8020000000000001E-2</v>
+      </c>
+      <c r="C11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12">
         <v>0.45100000000000001</v>
       </c>
-      <c r="B10">
-        <f t="shared" si="0"/>
+      <c r="B12">
+        <f>IF(A12&lt;0.4, A12 * 0.016 + 4 * 0.00001, A12 * 0.02 + 10 * 0.001)</f>
         <v>1.9020000000000002E-2</v>
       </c>
-      <c r="C10">
+      <c r="C12">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13">
         <v>0.499</v>
       </c>
-      <c r="B11">
-        <f t="shared" si="0"/>
+      <c r="B13">
+        <f>IF(A13&lt;0.4, A13 * 0.016 + 4 * 0.00001, A13 * 0.02 + 10 * 0.001)</f>
         <v>1.9980000000000001E-2</v>
       </c>
-      <c r="C11">
+      <c r="C13">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14">
         <v>0.54900000000000004</v>
       </c>
-      <c r="B12">
-        <f t="shared" si="0"/>
+      <c r="B14">
+        <f>IF(A14&lt;0.4, A14 * 0.016 + 4 * 0.00001, A14 * 0.02 + 10 * 0.001)</f>
         <v>2.0980000000000002E-2</v>
       </c>
-      <c r="C12">
+      <c r="C14">
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15">
         <v>0.6</v>
       </c>
-      <c r="B13">
-        <f t="shared" si="0"/>
+      <c r="B15">
+        <f>IF(A15&lt;0.4, A15 * 0.016 + 4 * 0.00001, A15 * 0.02 + 10 * 0.001)</f>
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="C13">
+      <c r="C15">
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16">
         <v>0.64900000000000002</v>
       </c>
-      <c r="B14">
-        <f t="shared" si="0"/>
+      <c r="B16">
+        <f>IF(A16&lt;0.4, A16 * 0.016 + 4 * 0.00001, A16 * 0.02 + 10 * 0.001)</f>
         <v>2.298E-2</v>
       </c>
-      <c r="C14">
+      <c r="C16">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17">
         <v>0.7</v>
       </c>
-      <c r="B15">
-        <f t="shared" si="0"/>
+      <c r="B17">
+        <f>IF(A17&lt;0.4, A17 * 0.016 + 4 * 0.00001, A17 * 0.02 + 10 * 0.001)</f>
         <v>2.4E-2</v>
       </c>
-      <c r="C15">
+      <c r="C17">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18">
         <v>0.749</v>
       </c>
-      <c r="B16">
-        <f t="shared" si="0"/>
+      <c r="B18">
+        <f>IF(A18&lt;0.4, A18 * 0.016 + 4 * 0.00001, A18 * 0.02 + 10 * 0.001)</f>
         <v>2.4980000000000002E-2</v>
       </c>
-      <c r="C16">
+      <c r="C18">
         <v>17</v>
       </c>
     </row>

</xml_diff>